<commit_message>
tbl_user_tokens created and deleted in scripts, docs also updated
</commit_message>
<xml_diff>
--- a/docs/tbl_user_token_design.xlsx
+++ b/docs/tbl_user_token_design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Projects\falcon-amazon\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jumarsolutionsltd-my.sharepoint.com/personal/will_pennell_jumar_co_uk/Documents/Documents/Documents/Projects/falcon-amazon/project/master_repo/falcon-amazon/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F152140-C6BA-43C4-9238-FE427EFE9526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{5F152140-C6BA-43C4-9238-FE427EFE9526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F19E5193-0538-4C01-B46F-B3561E48DE88}"/>
   <bookViews>
-    <workbookView xWindow="23085" yWindow="2880" windowWidth="14100" windowHeight="11325" xr2:uid="{E7F91725-D7C1-45A0-9574-7131905FAD8B}"/>
+    <workbookView xWindow="21795" yWindow="2505" windowWidth="15630" windowHeight="11325" xr2:uid="{E7F91725-D7C1-45A0-9574-7131905FAD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_user_token" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Field name</t>
   </si>
@@ -74,10 +74,16 @@
     <t>yes</t>
   </si>
   <si>
-    <t>uuid</t>
-  </si>
-  <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>uniqueidentifier</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>FK</t>
   </si>
 </sst>
 </file>
@@ -117,54 +123,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -176,39 +138,31 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,85 +477,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE8E9C2-4697-4FF0-9162-EF0DE2D5E8F8}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
+      <c r="A2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>